<commit_message>
TFS 251094 - update the Excel showcase application to include conditional formatting and "real data"
</commit_message>
<xml_diff>
--- a/Applications/IGExcel/IGExcel/IgExcel/DocumentTemplates/en/ProjectBudget.xlsx
+++ b/Applications/IGExcel/IGExcel/IgExcel/DocumentTemplates/en/ProjectBudget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\NetAdvantage\DEV\XAML\2014.2\Samples\XAML\Showcase.Apps\IGExcel.WPF\IgExcel\DocumentTemplates\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agoldenbaum\GitSamples\wpf-samples\Applications\IGExcel\IGExcel\IgExcel\DocumentTemplates\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,12 +24,12 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Data Worksheet'!$4:$4</definedName>
     <definedName name="TestTotal">'Expenditures Over Time'!$D$44</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>Develop Functional Specifications</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Expenditures Over Time</t>
   </si>
   <si>
-    <t>Other cost</t>
-  </si>
-  <si>
     <t>PROJECT TASKS</t>
   </si>
   <si>
@@ -191,10 +188,6 @@
   </si>
   <si>
     <t>Project Data Worksheet</t>
-  </si>
-  <si>
-    <t>OTHER
- COST</t>
   </si>
   <si>
     <t>PROJECT
@@ -219,7 +212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
@@ -947,7 +940,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1033,9 +1026,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1070,15 +1060,6 @@
     <xf numFmtId="164" fontId="11" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1297,9 +1278,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="42" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1822,7 +1800,9 @@
   </sheetPr>
   <dimension ref="B1:I44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1834,26 +1814,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+        <v>27</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11"/>
@@ -1862,27 +1842,27 @@
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="50"/>
-      <c r="C4" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="52" t="s">
+      <c r="B4" s="46"/>
+      <c r="C4" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="F4" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="G4" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="52" t="s">
+      <c r="H4" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="I4" s="48" t="s">
         <v>33</v>
-      </c>
-      <c r="I4" s="52" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1896,160 +1876,165 @@
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="116" t="s">
-        <v>58</v>
+      <c r="B6" s="112" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E6" s="22">
-        <v>1</v>
+        <f>PRODUCT(D6, 25)</f>
+        <v>250</v>
       </c>
       <c r="F6" s="22">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G6" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="22">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I6" s="23">
-        <f t="shared" ref="I6:I11" si="0">SUM(D6:H6)</f>
-        <v>5</v>
+        <f t="shared" ref="I6:I11" si="0">SUM(E6:H6)</f>
+        <v>370</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="116"/>
+      <c r="B7" s="112"/>
       <c r="C7" s="20" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="21">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E7" s="22">
-        <v>1</v>
+        <f>PRODUCT(D7, 25)</f>
+        <v>750</v>
       </c>
       <c r="F7" s="22">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="G7" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="22">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="I7" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="116"/>
+      <c r="B8" s="112"/>
       <c r="C8" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E8" s="22">
-        <v>1</v>
+        <f>PRODUCT(D8, 25)</f>
+        <v>250</v>
       </c>
       <c r="F8" s="22">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="G8" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="22">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I8" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="116"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="21">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E9" s="22">
-        <v>1</v>
+        <f>PRODUCT(D9, 25)</f>
+        <v>375</v>
       </c>
       <c r="F9" s="22">
-        <v>1</v>
+        <v>320</v>
       </c>
       <c r="G9" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="22">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="I9" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>765</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="116"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="20" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="21">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E10" s="22">
-        <v>1</v>
+        <f>PRODUCT(D10, 25)</f>
+        <v>250</v>
       </c>
       <c r="F10" s="22">
-        <v>1</v>
+        <v>115</v>
       </c>
       <c r="G10" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="22">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="I10" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="116"/>
-      <c r="C11" s="34" t="s">
+      <c r="B11" s="112"/>
+      <c r="C11" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="35">
+      <c r="D11" s="34">
         <f>SUM(D6:D10)</f>
-        <v>5</v>
-      </c>
-      <c r="E11" s="36">
+        <v>75</v>
+      </c>
+      <c r="E11" s="35">
         <f>SUM(E6:E10)</f>
-        <v>5</v>
-      </c>
-      <c r="F11" s="36">
+        <v>1875</v>
+      </c>
+      <c r="F11" s="35">
         <f>SUM(F6:F10)</f>
-        <v>5</v>
-      </c>
-      <c r="G11" s="36">
+        <v>1290</v>
+      </c>
+      <c r="G11" s="35">
         <f>SUM(G6:G10)</f>
-        <v>5</v>
-      </c>
-      <c r="H11" s="36">
+        <v>0</v>
+      </c>
+      <c r="H11" s="35">
         <f>SUM(H6:H10)</f>
-        <v>5</v>
-      </c>
-      <c r="I11" s="36">
+        <v>470</v>
+      </c>
+      <c r="I11" s="35">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2063,160 +2048,165 @@
       <c r="I12" s="27"/>
     </row>
     <row r="13" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="117" t="s">
-        <v>57</v>
+      <c r="B13" s="113" t="s">
+        <v>55</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="21">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E13" s="22">
-        <v>0</v>
+        <f>PRODUCT(D13, 25)</f>
+        <v>1000</v>
       </c>
       <c r="F13" s="22">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="G13" s="22">
         <v>0</v>
       </c>
       <c r="H13" s="22">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I13" s="23">
-        <f t="shared" ref="I13:I18" si="1">SUM(D13:H13)</f>
-        <v>0</v>
+        <f t="shared" ref="I13:I18" si="1">SUM(E13:H13)</f>
+        <v>1380</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="117"/>
+      <c r="B14" s="113"/>
       <c r="C14" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E14" s="22">
-        <v>0</v>
+        <f>PRODUCT(D14, 25)</f>
+        <v>250</v>
       </c>
       <c r="F14" s="22">
-        <v>0</v>
+        <v>850</v>
       </c>
       <c r="G14" s="22">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H14" s="22">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I14" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="117"/>
+      <c r="B15" s="113"/>
       <c r="C15" s="20" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E15" s="22">
-        <v>0</v>
+        <f>PRODUCT(D15, 25)</f>
+        <v>250</v>
       </c>
       <c r="F15" s="22">
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="G15" s="22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H15" s="22">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I15" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="117"/>
+      <c r="B16" s="113"/>
       <c r="C16" s="20" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E16" s="22">
-        <v>0</v>
+        <f>PRODUCT(D16, 25)</f>
+        <v>250</v>
       </c>
       <c r="F16" s="22">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="G16" s="22">
         <v>0</v>
       </c>
       <c r="H16" s="22">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I16" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>545</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="117"/>
+      <c r="B17" s="113"/>
       <c r="C17" s="20" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="21">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E17" s="22">
-        <v>0</v>
+        <f>PRODUCT(D17, 25)</f>
+        <v>625</v>
       </c>
       <c r="F17" s="22">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="G17" s="22">
         <v>0</v>
       </c>
       <c r="H17" s="22">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I17" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>915</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="117"/>
-      <c r="C18" s="37" t="s">
+      <c r="B18" s="113"/>
+      <c r="C18" s="36" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="24">
         <f>SUM(D13:D17)</f>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E18" s="25">
         <f>SUM(E13:E17)</f>
-        <v>0</v>
+        <v>2375</v>
       </c>
       <c r="F18" s="25">
         <f>SUM(F13:F17)</f>
-        <v>0</v>
+        <v>2480</v>
       </c>
       <c r="G18" s="25">
         <f>SUM(G13:G17)</f>
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="H18" s="25">
         <f>SUM(H13:H17)</f>
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="I18" s="25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5805</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2230,185 +2220,191 @@
       <c r="I19" s="29"/>
     </row>
     <row r="20" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="121" t="s">
-        <v>56</v>
+      <c r="B20" s="116" t="s">
+        <v>54</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E20" s="22">
-        <v>0</v>
+        <f t="shared" ref="E20:E25" si="2">PRODUCT(D20, 25)</f>
+        <v>250</v>
       </c>
       <c r="F20" s="22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G20" s="22">
         <v>0</v>
       </c>
       <c r="H20" s="22">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="I20" s="23">
-        <f t="shared" ref="I20:I26" si="2">SUM(D20:H20)</f>
-        <v>0</v>
+        <f t="shared" ref="I20:I26" si="3">SUM(E20:H20)</f>
+        <v>570</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="121"/>
+      <c r="B21" s="116"/>
       <c r="C21" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="21">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E21" s="22">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>500</v>
       </c>
       <c r="F21" s="22">
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="G21" s="22">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H21" s="22">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I21" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1280</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="121"/>
+      <c r="B22" s="116"/>
       <c r="C22" s="20" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E22" s="22">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>375</v>
       </c>
       <c r="F22" s="22">
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="G22" s="22">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H22" s="22">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I22" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1105</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="121"/>
+      <c r="B23" s="116"/>
       <c r="C23" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E23" s="22">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>125</v>
       </c>
       <c r="F23" s="22">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G23" s="22">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H23" s="22">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I23" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="121"/>
+      <c r="B24" s="116"/>
       <c r="C24" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E24" s="22">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>125</v>
       </c>
       <c r="F24" s="22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G24" s="22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H24" s="22">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I24" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="121"/>
+      <c r="B25" s="116"/>
       <c r="C25" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E25" s="22">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>375</v>
       </c>
       <c r="F25" s="22">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="G25" s="22">
         <v>0</v>
       </c>
       <c r="H25" s="22">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I25" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>685</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="121"/>
-      <c r="C26" s="38" t="s">
+      <c r="B26" s="116"/>
+      <c r="C26" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="38">
         <f>SUM(D20:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="40">
+        <v>70</v>
+      </c>
+      <c r="E26" s="39">
         <f>SUM(E20:E25)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="40">
+        <v>1750</v>
+      </c>
+      <c r="F26" s="39">
         <f>SUM(F20:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="40">
+        <v>1280</v>
+      </c>
+      <c r="G26" s="39">
         <f>SUM(G20:G25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="40">
+        <v>590</v>
+      </c>
+      <c r="H26" s="39">
         <f>SUM(H20:H25)</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="40">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>750</v>
+      </c>
+      <c r="I26" s="39">
+        <f t="shared" si="3"/>
+        <v>4370</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2422,438 +2418,342 @@
       <c r="I27" s="30"/>
     </row>
     <row r="28" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="122" t="s">
-        <v>55</v>
+      <c r="B28" s="117" t="s">
+        <v>53</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E28" s="22">
-        <v>0</v>
+        <f t="shared" ref="E28:E34" si="4">PRODUCT(D28, 25)</f>
+        <v>250</v>
       </c>
       <c r="F28" s="22">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="G28" s="22">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="H28" s="22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I28" s="23">
-        <f t="shared" ref="I28:I35" si="3">SUM(D28:H28)</f>
-        <v>0</v>
+        <f t="shared" ref="I28:I35" si="5">SUM(E28:H28)</f>
+        <v>920</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="122"/>
+      <c r="B29" s="117"/>
       <c r="C29" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E29" s="22">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>250</v>
       </c>
       <c r="F29" s="22">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="G29" s="22">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="H29" s="22">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I29" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>825</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="122"/>
+      <c r="B30" s="117"/>
       <c r="C30" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D30" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E30" s="22">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>375</v>
       </c>
       <c r="F30" s="22">
-        <v>0</v>
+        <v>520</v>
       </c>
       <c r="G30" s="22">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="H30" s="22">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="I30" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1290</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="122"/>
+      <c r="B31" s="117"/>
       <c r="C31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E31" s="22">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>250</v>
       </c>
       <c r="F31" s="22">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="G31" s="22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H31" s="22">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="I31" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>625</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="122"/>
+      <c r="B32" s="117"/>
       <c r="C32" s="20" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E32" s="22">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>250</v>
       </c>
       <c r="F32" s="22">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="G32" s="22">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="H32" s="22">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I32" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>770</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="122"/>
+      <c r="B33" s="117"/>
       <c r="C33" s="20" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E33" s="22">
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>375</v>
       </c>
       <c r="F33" s="22">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="G33" s="22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H33" s="22">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I33" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>915</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="122"/>
+      <c r="B34" s="117"/>
       <c r="C34" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="21">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E34" s="22">
-        <v>0</v>
+        <f>PRODUCT(D34, 25)</f>
+        <v>250</v>
       </c>
       <c r="F34" s="22">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="G34" s="22">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="H34" s="22">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I34" s="23">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>925</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="122"/>
-      <c r="C35" s="41" t="s">
+      <c r="B35" s="117"/>
+      <c r="C35" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="41">
         <f>SUM(D28:D34)</f>
-        <v>0</v>
-      </c>
-      <c r="E35" s="43">
+        <v>80</v>
+      </c>
+      <c r="E35" s="42">
         <f>SUM(E28:E34)</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="43">
+        <v>2000</v>
+      </c>
+      <c r="F35" s="42">
         <f>SUM(F28:F34)</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="43">
+        <v>2145</v>
+      </c>
+      <c r="G35" s="42">
         <f>SUM(G28:G34)</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="43">
+        <v>1430</v>
+      </c>
+      <c r="H35" s="42">
         <f>SUM(H28:H34)</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="43">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>695</v>
+      </c>
+      <c r="I35" s="42">
+        <f t="shared" si="5"/>
+        <v>6270</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="32"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
     </row>
     <row r="37" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="120" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="21">
-        <v>0</v>
-      </c>
-      <c r="E37" s="22">
-        <v>0</v>
-      </c>
-      <c r="F37" s="22">
-        <v>0</v>
-      </c>
-      <c r="G37" s="22">
-        <v>0</v>
-      </c>
-      <c r="H37" s="22">
-        <v>0</v>
-      </c>
-      <c r="I37" s="23">
-        <f>SUM(D37:H37)</f>
-        <v>0</v>
-      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="120"/>
-      <c r="C38" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="21">
-        <v>0</v>
-      </c>
-      <c r="E38" s="22">
-        <v>0</v>
-      </c>
-      <c r="F38" s="22">
-        <v>0</v>
-      </c>
-      <c r="G38" s="22">
-        <v>0</v>
-      </c>
-      <c r="H38" s="22">
-        <v>0</v>
-      </c>
-      <c r="I38" s="23">
-        <f>SUM(D38:H38)</f>
-        <v>0</v>
+      <c r="B38" s="114" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="114"/>
+      <c r="D38" s="105">
+        <f>SUM(E41,D35,D26,D18,D11)</f>
+        <v>320</v>
+      </c>
+      <c r="E38" s="106">
+        <f>SUM(E35,E26,E18,E11)</f>
+        <v>8000</v>
+      </c>
+      <c r="F38" s="106">
+        <f>SUM(F35,F26,F18,F11)</f>
+        <v>7195</v>
+      </c>
+      <c r="G38" s="106">
+        <f>SUM(G35,G26,G18,G11)</f>
+        <v>2440</v>
+      </c>
+      <c r="H38" s="106">
+        <f>SUM(H35,H26,H18,H11)</f>
+        <v>2445</v>
+      </c>
+      <c r="I38" s="103">
+        <f>SUM(I35,I26,I18,I11)</f>
+        <v>20080</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="120"/>
-      <c r="C39" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D39" s="21">
-        <v>0</v>
-      </c>
-      <c r="E39" s="22">
-        <v>0</v>
-      </c>
-      <c r="F39" s="22">
-        <v>0</v>
-      </c>
-      <c r="G39" s="22">
-        <v>0</v>
-      </c>
-      <c r="H39" s="22">
-        <v>0</v>
-      </c>
-      <c r="I39" s="23">
-        <f>SUM(D39:H39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="120"/>
-      <c r="C40" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="45">
-        <f>SUM(D37:D39)</f>
-        <v>0</v>
-      </c>
-      <c r="E40" s="46">
-        <f>SUM(E37:E39)</f>
-        <v>0</v>
-      </c>
-      <c r="F40" s="46">
-        <f>SUM(F37:F39)</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="46">
-        <f>SUM(G37:G39)</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="46">
-        <f>SUM(H37:H39)</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="46">
-        <f>SUM(D40:H40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="118" t="s">
+      <c r="B39" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="118"/>
-      <c r="D42" s="109">
-        <f>SUM(D40,D35,D26,D18,D11)</f>
-        <v>5</v>
-      </c>
-      <c r="E42" s="110">
-        <f t="shared" ref="E42:I42" si="4">SUM(E40,E35,E26,E18,E11)</f>
-        <v>5</v>
-      </c>
-      <c r="F42" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="G42" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="H42" s="110">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="I42" s="107">
-        <f t="shared" si="4"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="107">
+        <v>10</v>
+      </c>
+      <c r="E39" s="108">
+        <f>PRODUCT(D39, 25)</f>
+        <v>250</v>
+      </c>
+      <c r="F39" s="108">
+        <v>200</v>
+      </c>
+      <c r="G39" s="108">
+        <v>0</v>
+      </c>
+      <c r="H39" s="108">
         <v>25</v>
       </c>
-    </row>
-    <row r="43" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="119" t="s">
+      <c r="I39" s="104">
+        <f>SUM(E39:H39)</f>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="119"/>
-      <c r="D43" s="111">
-        <v>0</v>
-      </c>
-      <c r="E43" s="112">
-        <v>0</v>
-      </c>
-      <c r="F43" s="112">
-        <v>0</v>
-      </c>
-      <c r="G43" s="112">
-        <v>0</v>
-      </c>
-      <c r="H43" s="112">
-        <v>0</v>
-      </c>
-      <c r="I43" s="108">
-        <f>SUM(E43:H43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="118"/>
-      <c r="D44" s="109">
-        <f>SUM(D42:D43)</f>
-        <v>5</v>
-      </c>
-      <c r="E44" s="110">
-        <f t="shared" ref="E44:H44" si="5">SUM(E42:E43)</f>
-        <v>5</v>
-      </c>
-      <c r="F44" s="110">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="G44" s="110">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="H44" s="110">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I44" s="107">
-        <f>SUM(I42:I43)</f>
-        <v>25</v>
-      </c>
-    </row>
+      <c r="C40" s="114"/>
+      <c r="D40" s="105">
+        <f>SUM(D38:D39)</f>
+        <v>330</v>
+      </c>
+      <c r="E40" s="106">
+        <f t="shared" ref="E40:H40" si="6">SUM(E38:E39)</f>
+        <v>8250</v>
+      </c>
+      <c r="F40" s="106">
+        <f t="shared" si="6"/>
+        <v>7395</v>
+      </c>
+      <c r="G40" s="106">
+        <f t="shared" si="6"/>
+        <v>2440</v>
+      </c>
+      <c r="H40" s="106">
+        <f t="shared" si="6"/>
+        <v>2470</v>
+      </c>
+      <c r="I40" s="103">
+        <f>SUM(I38:I39)</f>
+        <v>20555</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="B13:B18"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B37:B40"/>
     <mergeCell ref="B20:B26"/>
     <mergeCell ref="B28:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I43" formulaRange="1"/>
+    <ignoredError sqref="I39 I28:I34 I20:I25 I13:I17 I6:I10" formulaRange="1"/>
   </ignoredErrors>
   <picture r:id="rId2"/>
 </worksheet>
@@ -2866,7 +2766,9 @@
   </sheetPr>
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2880,48 +2782,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="11"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="49"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="47"/>
-      <c r="C4" s="55" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="E4" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="F4" s="54" t="s">
         <v>40</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2931,84 +2833,84 @@
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="124" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="81" t="s">
+      <c r="B6" s="119" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="82">
-        <v>0</v>
-      </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
+      <c r="D6" s="78">
+        <v>0</v>
+      </c>
+      <c r="E6" s="79"/>
+      <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="125"/>
-      <c r="C7" s="85" t="s">
+      <c r="B7" s="120"/>
+      <c r="C7" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="86">
-        <v>0</v>
-      </c>
-      <c r="E7" s="87"/>
-      <c r="F7" s="88"/>
+      <c r="D7" s="82">
+        <v>0</v>
+      </c>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
     </row>
     <row r="8" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="125"/>
-      <c r="C8" s="85" t="s">
+      <c r="B8" s="120"/>
+      <c r="C8" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="86">
-        <v>0</v>
-      </c>
-      <c r="E8" s="87"/>
-      <c r="F8" s="88"/>
+      <c r="D8" s="82">
+        <v>0</v>
+      </c>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
     </row>
     <row r="9" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="125"/>
-      <c r="C9" s="85" t="s">
+      <c r="B9" s="120"/>
+      <c r="C9" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="86">
-        <v>0</v>
-      </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="88"/>
+      <c r="D9" s="82">
+        <v>0</v>
+      </c>
+      <c r="E9" s="83"/>
+      <c r="F9" s="84"/>
     </row>
     <row r="10" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="125"/>
-      <c r="C10" s="85" t="s">
+      <c r="B10" s="120"/>
+      <c r="C10" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="86">
-        <v>0</v>
-      </c>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
+      <c r="D10" s="82">
+        <v>0</v>
+      </c>
+      <c r="E10" s="83"/>
+      <c r="F10" s="84"/>
     </row>
     <row r="11" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="125"/>
-      <c r="C11" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="86">
-        <v>0</v>
-      </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="82">
+        <v>0</v>
+      </c>
+      <c r="E11" s="83"/>
+      <c r="F11" s="84"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="126"/>
-      <c r="C12" s="59" t="s">
+      <c r="B12" s="121"/>
+      <c r="C12" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="56">
         <f>SUM(D6:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
@@ -3017,84 +2919,84 @@
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="127" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="89" t="s">
+      <c r="B14" s="122" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="90">
-        <v>0</v>
-      </c>
-      <c r="E14" s="91"/>
-      <c r="F14" s="92"/>
+      <c r="D14" s="86">
+        <v>0</v>
+      </c>
+      <c r="E14" s="87"/>
+      <c r="F14" s="88"/>
     </row>
     <row r="15" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="128"/>
-      <c r="C15" s="85" t="s">
+      <c r="B15" s="123"/>
+      <c r="C15" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="86">
-        <v>0</v>
-      </c>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
+      <c r="D15" s="82">
+        <v>0</v>
+      </c>
+      <c r="E15" s="83"/>
+      <c r="F15" s="84"/>
     </row>
     <row r="16" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="128"/>
-      <c r="C16" s="85" t="s">
+      <c r="B16" s="123"/>
+      <c r="C16" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="86">
-        <v>0</v>
-      </c>
-      <c r="E16" s="87"/>
-      <c r="F16" s="88"/>
+      <c r="D16" s="82">
+        <v>0</v>
+      </c>
+      <c r="E16" s="83"/>
+      <c r="F16" s="84"/>
     </row>
     <row r="17" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="128"/>
-      <c r="C17" s="85" t="s">
+      <c r="B17" s="123"/>
+      <c r="C17" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="86">
-        <v>0</v>
-      </c>
-      <c r="E17" s="87"/>
-      <c r="F17" s="88"/>
+      <c r="D17" s="82">
+        <v>0</v>
+      </c>
+      <c r="E17" s="83"/>
+      <c r="F17" s="84"/>
     </row>
     <row r="18" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="128"/>
-      <c r="C18" s="85" t="s">
+      <c r="B18" s="123"/>
+      <c r="C18" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="86">
-        <v>0</v>
-      </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="88"/>
+      <c r="D18" s="82">
+        <v>0</v>
+      </c>
+      <c r="E18" s="83"/>
+      <c r="F18" s="84"/>
     </row>
     <row r="19" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="128"/>
-      <c r="C19" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="86">
-        <v>0</v>
-      </c>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88"/>
+      <c r="B19" s="123"/>
+      <c r="C19" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="82">
+        <v>0</v>
+      </c>
+      <c r="E19" s="83"/>
+      <c r="F19" s="84"/>
     </row>
     <row r="20" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="129"/>
-      <c r="C20" s="63" t="s">
+      <c r="B20" s="124"/>
+      <c r="C20" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="60">
         <f>SUM(D14:D19)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
@@ -3103,84 +3005,84 @@
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="130" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="93" t="s">
+      <c r="B22" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="94">
-        <v>0</v>
-      </c>
-      <c r="E22" s="95"/>
-      <c r="F22" s="96"/>
+      <c r="D22" s="90">
+        <v>0</v>
+      </c>
+      <c r="E22" s="91"/>
+      <c r="F22" s="92"/>
     </row>
     <row r="23" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="131"/>
-      <c r="C23" s="85" t="s">
+      <c r="B23" s="126"/>
+      <c r="C23" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="86">
-        <v>0</v>
-      </c>
-      <c r="E23" s="87"/>
-      <c r="F23" s="88"/>
+      <c r="D23" s="82">
+        <v>0</v>
+      </c>
+      <c r="E23" s="83"/>
+      <c r="F23" s="84"/>
     </row>
     <row r="24" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="131"/>
-      <c r="C24" s="85" t="s">
+      <c r="B24" s="126"/>
+      <c r="C24" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="86">
-        <v>0</v>
-      </c>
-      <c r="E24" s="87"/>
-      <c r="F24" s="88"/>
+      <c r="D24" s="82">
+        <v>0</v>
+      </c>
+      <c r="E24" s="83"/>
+      <c r="F24" s="84"/>
     </row>
     <row r="25" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="131"/>
-      <c r="C25" s="85" t="s">
+      <c r="B25" s="126"/>
+      <c r="C25" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="86">
-        <v>0</v>
-      </c>
-      <c r="E25" s="87"/>
-      <c r="F25" s="88"/>
+      <c r="D25" s="82">
+        <v>0</v>
+      </c>
+      <c r="E25" s="83"/>
+      <c r="F25" s="84"/>
     </row>
     <row r="26" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="131"/>
-      <c r="C26" s="85" t="s">
+      <c r="B26" s="126"/>
+      <c r="C26" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="86">
-        <v>0</v>
-      </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="88"/>
+      <c r="D26" s="82">
+        <v>0</v>
+      </c>
+      <c r="E26" s="83"/>
+      <c r="F26" s="84"/>
     </row>
     <row r="27" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="131"/>
-      <c r="C27" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="86">
-        <v>0</v>
-      </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="88"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="82">
+        <v>0</v>
+      </c>
+      <c r="E27" s="83"/>
+      <c r="F27" s="84"/>
     </row>
     <row r="28" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="132"/>
-      <c r="C28" s="67" t="s">
+      <c r="B28" s="127"/>
+      <c r="C28" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="64">
         <f>SUM(D22:D27)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="70"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="66"/>
     </row>
     <row r="29" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C29" s="7"/>
@@ -3189,84 +3091,84 @@
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="133" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="97" t="s">
+      <c r="B30" s="128" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="98">
-        <v>0</v>
-      </c>
-      <c r="E30" s="99"/>
-      <c r="F30" s="100"/>
+      <c r="D30" s="94">
+        <v>0</v>
+      </c>
+      <c r="E30" s="95"/>
+      <c r="F30" s="96"/>
     </row>
     <row r="31" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="134"/>
-      <c r="C31" s="85" t="s">
+      <c r="B31" s="129"/>
+      <c r="C31" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="86">
-        <v>0</v>
-      </c>
-      <c r="E31" s="87"/>
-      <c r="F31" s="88"/>
+      <c r="D31" s="82">
+        <v>0</v>
+      </c>
+      <c r="E31" s="83"/>
+      <c r="F31" s="84"/>
     </row>
     <row r="32" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="134"/>
-      <c r="C32" s="85" t="s">
+      <c r="B32" s="129"/>
+      <c r="C32" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="86">
-        <v>0</v>
-      </c>
-      <c r="E32" s="87"/>
-      <c r="F32" s="88"/>
+      <c r="D32" s="82">
+        <v>0</v>
+      </c>
+      <c r="E32" s="83"/>
+      <c r="F32" s="84"/>
     </row>
     <row r="33" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="134"/>
-      <c r="C33" s="85" t="s">
+      <c r="B33" s="129"/>
+      <c r="C33" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="86">
-        <v>0</v>
-      </c>
-      <c r="E33" s="87"/>
-      <c r="F33" s="88"/>
+      <c r="D33" s="82">
+        <v>0</v>
+      </c>
+      <c r="E33" s="83"/>
+      <c r="F33" s="84"/>
     </row>
     <row r="34" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="134"/>
-      <c r="C34" s="85" t="s">
+      <c r="B34" s="129"/>
+      <c r="C34" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="86">
-        <v>0</v>
-      </c>
-      <c r="E34" s="87"/>
-      <c r="F34" s="88"/>
+      <c r="D34" s="82">
+        <v>0</v>
+      </c>
+      <c r="E34" s="83"/>
+      <c r="F34" s="84"/>
     </row>
     <row r="35" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="134"/>
-      <c r="C35" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="86">
-        <v>0</v>
-      </c>
-      <c r="E35" s="87"/>
-      <c r="F35" s="88"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="82">
+        <v>0</v>
+      </c>
+      <c r="E35" s="83"/>
+      <c r="F35" s="84"/>
     </row>
     <row r="36" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="135"/>
-      <c r="C36" s="71" t="s">
+      <c r="B36" s="130"/>
+      <c r="C36" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="72">
+      <c r="D36" s="68">
         <f>SUM(D30:D35)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="73"/>
-      <c r="F36" s="74"/>
+      <c r="E36" s="69"/>
+      <c r="F36" s="70"/>
     </row>
     <row r="37" spans="2:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C37" s="7"/>
@@ -3275,84 +3177,84 @@
       <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="136" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="106" t="s">
+      <c r="B38" s="131" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="101">
-        <v>0</v>
-      </c>
-      <c r="E38" s="102"/>
-      <c r="F38" s="103"/>
+      <c r="D38" s="97">
+        <v>0</v>
+      </c>
+      <c r="E38" s="98"/>
+      <c r="F38" s="99"/>
     </row>
     <row r="39" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="137"/>
-      <c r="C39" s="85" t="s">
+      <c r="B39" s="132"/>
+      <c r="C39" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="86">
-        <v>0</v>
-      </c>
-      <c r="E39" s="87"/>
-      <c r="F39" s="88"/>
+      <c r="D39" s="82">
+        <v>0</v>
+      </c>
+      <c r="E39" s="83"/>
+      <c r="F39" s="84"/>
     </row>
     <row r="40" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="137"/>
-      <c r="C40" s="85" t="s">
+      <c r="B40" s="132"/>
+      <c r="C40" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="86">
-        <v>0</v>
-      </c>
-      <c r="E40" s="87"/>
-      <c r="F40" s="88"/>
+      <c r="D40" s="82">
+        <v>0</v>
+      </c>
+      <c r="E40" s="83"/>
+      <c r="F40" s="84"/>
     </row>
     <row r="41" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="137"/>
-      <c r="C41" s="85" t="s">
+      <c r="B41" s="132"/>
+      <c r="C41" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="86">
-        <v>0</v>
-      </c>
-      <c r="E41" s="87"/>
-      <c r="F41" s="88"/>
+      <c r="D41" s="82">
+        <v>0</v>
+      </c>
+      <c r="E41" s="83"/>
+      <c r="F41" s="84"/>
     </row>
     <row r="42" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="137"/>
-      <c r="C42" s="85" t="s">
+      <c r="B42" s="132"/>
+      <c r="C42" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="86">
-        <v>0</v>
-      </c>
-      <c r="E42" s="87"/>
-      <c r="F42" s="88"/>
+      <c r="D42" s="82">
+        <v>0</v>
+      </c>
+      <c r="E42" s="83"/>
+      <c r="F42" s="84"/>
     </row>
     <row r="43" spans="2:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="137"/>
-      <c r="C43" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="86">
-        <v>0</v>
-      </c>
-      <c r="E43" s="87"/>
-      <c r="F43" s="88"/>
+      <c r="B43" s="132"/>
+      <c r="C43" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" s="82">
+        <v>0</v>
+      </c>
+      <c r="E43" s="83"/>
+      <c r="F43" s="84"/>
     </row>
     <row r="44" spans="2:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="138"/>
-      <c r="C44" s="105" t="s">
+      <c r="B44" s="133"/>
+      <c r="C44" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="75">
+      <c r="D44" s="71">
         <f>SUM(D38:D43)</f>
         <v>0</v>
       </c>
-      <c r="E44" s="76"/>
-      <c r="F44" s="77"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="73"/>
     </row>
     <row r="45" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C45" s="7"/>
@@ -3361,16 +3263,16 @@
       <c r="F45" s="6"/>
     </row>
     <row r="46" spans="2:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="123" t="s">
+      <c r="B46" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="123"/>
-      <c r="D46" s="115">
+      <c r="C46" s="118"/>
+      <c r="D46" s="111">
         <f>SUM(TestTotal,ConstructionTotal,Planning2Total,PlanningTotal,InstallTotal)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="113"/>
-      <c r="F46" s="114"/>
+      <c r="E46" s="109"/>
+      <c r="F46" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3408,46 +3310,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="53"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="49"/>
       <c r="G1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+        <v>52</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="14">
         <v>1</v>
       </c>
@@ -3465,25 +3367,25 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="80"/>
-      <c r="B6" s="78">
+      <c r="A6" s="76"/>
+      <c r="B6" s="74">
         <v>2</v>
       </c>
-      <c r="C6" s="79">
+      <c r="C6" s="75">
         <v>1480</v>
       </c>
-      <c r="D6" s="79">
+      <c r="D6" s="75">
         <v>3190</v>
       </c>
-      <c r="E6" s="79">
+      <c r="E6" s="75">
         <v>1490</v>
       </c>
-      <c r="F6" s="79">
+      <c r="F6" s="75">
         <v>2950</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="80"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="14">
         <v>3</v>
       </c>
@@ -3501,25 +3403,25 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="80"/>
-      <c r="B8" s="78">
+      <c r="A8" s="76"/>
+      <c r="B8" s="74">
         <v>4</v>
       </c>
-      <c r="C8" s="79">
+      <c r="C8" s="75">
         <v>4030</v>
       </c>
-      <c r="D8" s="79">
+      <c r="D8" s="75">
         <v>1370</v>
       </c>
-      <c r="E8" s="79">
+      <c r="E8" s="75">
         <v>1590</v>
       </c>
-      <c r="F8" s="79">
+      <c r="F8" s="75">
         <v>2330</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="14">
         <v>5</v>
       </c>
@@ -3537,25 +3439,25 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="80"/>
-      <c r="B10" s="78">
+      <c r="A10" s="76"/>
+      <c r="B10" s="74">
         <v>6</v>
       </c>
-      <c r="C10" s="79">
+      <c r="C10" s="75">
         <v>2480</v>
       </c>
-      <c r="D10" s="79">
+      <c r="D10" s="75">
         <v>1180</v>
       </c>
-      <c r="E10" s="79">
+      <c r="E10" s="75">
         <v>3430</v>
       </c>
-      <c r="F10" s="79">
+      <c r="F10" s="75">
         <v>1840</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="80"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="14">
         <v>7</v>
       </c>
@@ -3573,25 +3475,25 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="80"/>
-      <c r="B12" s="78">
+      <c r="A12" s="76"/>
+      <c r="B12" s="74">
         <v>8</v>
       </c>
-      <c r="C12" s="79">
+      <c r="C12" s="75">
         <v>2160</v>
       </c>
-      <c r="D12" s="79">
+      <c r="D12" s="75">
         <v>4040</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E12" s="75">
         <v>3330</v>
       </c>
-      <c r="F12" s="79">
+      <c r="F12" s="75">
         <v>3300</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="80"/>
+      <c r="A13" s="76"/>
       <c r="B13" s="14">
         <v>9</v>
       </c>
@@ -3609,25 +3511,25 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="80"/>
-      <c r="B14" s="78">
+      <c r="A14" s="76"/>
+      <c r="B14" s="74">
         <v>10</v>
       </c>
-      <c r="C14" s="79">
+      <c r="C14" s="75">
         <v>2300</v>
       </c>
-      <c r="D14" s="79">
+      <c r="D14" s="75">
         <v>1140</v>
       </c>
-      <c r="E14" s="79">
+      <c r="E14" s="75">
         <v>2450</v>
       </c>
-      <c r="F14" s="79">
+      <c r="F14" s="75">
         <v>2990</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="80"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="14">
         <v>11</v>
       </c>
@@ -3645,25 +3547,25 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="80"/>
-      <c r="B16" s="78">
+      <c r="A16" s="76"/>
+      <c r="B16" s="74">
         <v>12</v>
       </c>
-      <c r="C16" s="79">
+      <c r="C16" s="75">
         <v>2300</v>
       </c>
-      <c r="D16" s="79">
+      <c r="D16" s="75">
         <v>3910</v>
       </c>
-      <c r="E16" s="79">
+      <c r="E16" s="75">
         <v>1330</v>
       </c>
-      <c r="F16" s="79">
+      <c r="F16" s="75">
         <v>2230</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="80"/>
+      <c r="A17" s="76"/>
       <c r="B17" s="14">
         <v>13</v>
       </c>
@@ -3681,25 +3583,25 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="78">
+      <c r="A18" s="76"/>
+      <c r="B18" s="74">
         <v>14</v>
       </c>
-      <c r="C18" s="79">
+      <c r="C18" s="75">
         <v>3140</v>
       </c>
-      <c r="D18" s="79">
+      <c r="D18" s="75">
         <v>3850</v>
       </c>
-      <c r="E18" s="79">
+      <c r="E18" s="75">
         <v>1580</v>
       </c>
-      <c r="F18" s="79">
+      <c r="F18" s="75">
         <v>1500</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="14">
         <v>15</v>
       </c>
@@ -3717,25 +3619,25 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="80"/>
-      <c r="B20" s="78">
+      <c r="A20" s="76"/>
+      <c r="B20" s="74">
         <v>16</v>
       </c>
-      <c r="C20" s="79">
+      <c r="C20" s="75">
         <v>2060</v>
       </c>
-      <c r="D20" s="79">
+      <c r="D20" s="75">
         <v>3700</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E20" s="75">
         <v>1320</v>
       </c>
-      <c r="F20" s="79">
+      <c r="F20" s="75">
         <v>2590</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="80"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="14">
         <v>17</v>
       </c>
@@ -3753,25 +3655,25 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="80"/>
-      <c r="B22" s="78">
+      <c r="A22" s="76"/>
+      <c r="B22" s="74">
         <v>18</v>
       </c>
-      <c r="C22" s="79">
+      <c r="C22" s="75">
         <v>3740</v>
       </c>
-      <c r="D22" s="79">
+      <c r="D22" s="75">
         <v>1870</v>
       </c>
-      <c r="E22" s="79">
+      <c r="E22" s="75">
         <v>3480</v>
       </c>
-      <c r="F22" s="79">
+      <c r="F22" s="75">
         <v>3660</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="80"/>
+      <c r="A23" s="76"/>
       <c r="B23" s="14">
         <v>19</v>
       </c>
@@ -3789,25 +3691,25 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="80"/>
-      <c r="B24" s="78">
+      <c r="A24" s="76"/>
+      <c r="B24" s="74">
         <v>20</v>
       </c>
-      <c r="C24" s="79">
+      <c r="C24" s="75">
         <v>3230</v>
       </c>
-      <c r="D24" s="79">
+      <c r="D24" s="75">
         <v>2790</v>
       </c>
-      <c r="E24" s="79">
+      <c r="E24" s="75">
         <v>3710</v>
       </c>
-      <c r="F24" s="79">
+      <c r="F24" s="75">
         <v>2190</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="80"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="14">
         <v>21</v>
       </c>
@@ -3825,25 +3727,25 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="80"/>
-      <c r="B26" s="78">
+      <c r="A26" s="76"/>
+      <c r="B26" s="74">
         <v>22</v>
       </c>
-      <c r="C26" s="79">
+      <c r="C26" s="75">
         <v>1260</v>
       </c>
-      <c r="D26" s="79">
+      <c r="D26" s="75">
         <v>3890</v>
       </c>
-      <c r="E26" s="79">
+      <c r="E26" s="75">
         <v>2620</v>
       </c>
-      <c r="F26" s="79">
+      <c r="F26" s="75">
         <v>2470</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="80"/>
+      <c r="A27" s="76"/>
       <c r="B27" s="14">
         <v>23</v>
       </c>
@@ -3861,20 +3763,20 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="80"/>
-      <c r="B28" s="78">
+      <c r="A28" s="76"/>
+      <c r="B28" s="74">
         <v>24</v>
       </c>
-      <c r="C28" s="79">
+      <c r="C28" s="75">
         <v>2880</v>
       </c>
-      <c r="D28" s="79">
+      <c r="D28" s="75">
         <v>1740</v>
       </c>
-      <c r="E28" s="79">
+      <c r="E28" s="75">
         <v>2220</v>
       </c>
-      <c r="F28" s="79">
+      <c r="F28" s="75">
         <v>2140</v>
       </c>
     </row>

</xml_diff>